<commit_message>
updated trait scoring based on expert feedback
Former-commit-id: ed458eac03fc4439a0cf0aa6a74095110d4ec0f4
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/trait_val_key.xlsx
+++ b/_raw_data/xlsx/trait_val_key.xlsx
@@ -246,9 +246,6 @@
     <t>sensitive/not sensitive/NA (e.g. sea grass/limpet/whale)</t>
   </si>
   <si>
-    <t>light dependence</t>
-  </si>
-  <si>
     <t>air-sea interface</t>
   </si>
   <si>
@@ -420,20 +417,6 @@
     <t>sessile; nearly sessile/sedentary; passive; vertical migrator; mobile resident; horizontal migrator; nomadic</t>
   </si>
   <si>
-    <r>
-      <t>&lt;1 day; &lt;1 week; &lt;1 month; &lt;4 months; 4 months -1yr; &gt;1yr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>; not larvae</t>
-    </r>
-  </si>
-  <si>
     <t>sexual dioecious; sexual hermaphrodite; asexual; colonial</t>
   </si>
   <si>
@@ -556,6 +539,23 @@
   </si>
   <si>
     <t>epipelagic; mesopelagic; bathypelagic; abyssopelagic; hadopelagic; atmosphere</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;1 day; &lt;1 week; &lt;1 month; &lt;4 months; 4 months -1yr; &gt;1yr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; not larvae;holoplankton</t>
+    </r>
+  </si>
+  <si>
+    <t>photosynthetic</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1092,18 +1092,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1112,19 +1112,19 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1150,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1159,10 +1159,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1198,13 +1198,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1219,10 +1219,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1234,7 +1234,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1246,7 +1246,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1258,12 +1258,12 @@
         <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
@@ -1284,7 +1284,7 @@
         <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1332,341 +1332,341 @@
         <v>36</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
+      <c r="B21" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
       <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2"/>
       <c r="B44" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:4">

</xml_diff>